<commit_message>
Enhance date filtering in By_Stage and Stage_to_Stage pages; add total calls and successful calls methods in TotalModel; update data handling in Totals page for improved comparison functionality.
</commit_message>
<xml_diff>
--- a/data/khloud reports.xlsx
+++ b/data/khloud reports.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1dc152c07513850c/Documents/GitHub/DataAnalyzer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1670" documentId="13_ncr:1_{400F4DCB-612B-46F1-BD96-90EED01F7942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9500A9DF-40DF-4337-B2C6-5C16A854C736}"/>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1130,7 +1130,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1228,7 +1228,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1272,14 +1272,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1288,7 +1284,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1602,9 +1597,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1642,7 +1637,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1748,7 +1743,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1890,7 +1885,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1901,25 +1896,25 @@
   <dimension ref="A1:O112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" customWidth="1"/>
+    <col min="1" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="37.44140625" customWidth="1"/>
     <col min="6" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="10" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="10" width="19.109375" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30.75">
+    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1966,7 +1961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1018</v>
       </c>
@@ -1980,7 +1975,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1019</v>
       </c>
@@ -1997,7 +1992,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1020</v>
       </c>
@@ -2012,7 +2007,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1021</v>
       </c>
@@ -2026,7 +2021,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1022</v>
       </c>
@@ -2043,7 +2038,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1024</v>
       </c>
@@ -2060,7 +2055,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1025</v>
       </c>
@@ -2074,7 +2069,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1026</v>
       </c>
@@ -2094,7 +2089,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1027</v>
       </c>
@@ -2108,7 +2103,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2001</v>
       </c>
@@ -2122,7 +2117,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2002</v>
       </c>
@@ -2136,7 +2131,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2005</v>
       </c>
@@ -2154,7 +2149,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2006</v>
       </c>
@@ -2171,7 +2166,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2007</v>
       </c>
@@ -2185,7 +2180,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2008</v>
       </c>
@@ -2205,7 +2200,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2009</v>
       </c>
@@ -2219,7 +2214,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2010</v>
       </c>
@@ -2233,7 +2228,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2011</v>
       </c>
@@ -2247,7 +2242,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2012</v>
       </c>
@@ -2261,7 +2256,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2013</v>
       </c>
@@ -2275,7 +2270,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2014</v>
       </c>
@@ -2286,7 +2281,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2015</v>
       </c>
@@ -2300,7 +2295,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2031</v>
       </c>
@@ -2317,7 +2312,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2033</v>
       </c>
@@ -2334,7 +2329,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2035</v>
       </c>
@@ -2352,7 +2347,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2036</v>
       </c>
@@ -2366,7 +2361,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2037</v>
       </c>
@@ -2380,7 +2375,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -2394,7 +2389,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2038</v>
       </c>
@@ -2411,7 +2406,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2039</v>
       </c>
@@ -2428,7 +2423,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2040</v>
       </c>
@@ -2448,7 +2443,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2041</v>
       </c>
@@ -2465,7 +2460,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2042</v>
       </c>
@@ -2479,7 +2474,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="30.75">
+    <row r="35" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2043</v>
       </c>
@@ -2502,7 +2497,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2044</v>
       </c>
@@ -2519,7 +2514,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="30.75">
+    <row r="37" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2045</v>
       </c>
@@ -2539,7 +2534,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2046</v>
       </c>
@@ -2553,7 +2548,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2047</v>
       </c>
@@ -2570,7 +2565,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2048</v>
       </c>
@@ -2584,7 +2579,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2049</v>
       </c>
@@ -2598,7 +2593,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2050</v>
       </c>
@@ -2612,7 +2607,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2051</v>
       </c>
@@ -2626,7 +2621,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2052</v>
       </c>
@@ -2643,7 +2638,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2053</v>
       </c>
@@ -2660,7 +2655,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2054</v>
       </c>
@@ -2677,7 +2672,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2055</v>
       </c>
@@ -2694,7 +2689,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2056</v>
       </c>
@@ -2708,7 +2703,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2057</v>
       </c>
@@ -2722,7 +2717,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2058</v>
       </c>
@@ -2736,7 +2731,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2059</v>
       </c>
@@ -2750,7 +2745,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2060</v>
       </c>
@@ -2764,7 +2759,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2061</v>
       </c>
@@ -2781,7 +2776,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2062</v>
       </c>
@@ -2798,7 +2793,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2063</v>
       </c>
@@ -2821,7 +2816,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2064</v>
       </c>
@@ -2835,7 +2830,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2065</v>
       </c>
@@ -2849,7 +2844,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2066</v>
       </c>
@@ -2863,7 +2858,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2067</v>
       </c>
@@ -2880,7 +2875,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2068</v>
       </c>
@@ -2897,7 +2892,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2069</v>
       </c>
@@ -2926,7 +2921,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>75</v>
       </c>
@@ -2937,7 +2932,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>76</v>
       </c>
@@ -2948,7 +2943,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>77</v>
       </c>
@@ -2962,7 +2957,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="65" spans="2:6">
+    <row r="65" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>78</v>
       </c>
@@ -2973,7 +2968,7 @@
         <v>45907</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="15" customHeight="1">
+    <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>79</v>
       </c>
@@ -2984,7 +2979,7 @@
         <v>45938</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="15" customHeight="1">
+    <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>80</v>
       </c>
@@ -2995,7 +2990,7 @@
         <v>45937</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="15" customHeight="1">
+    <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>81</v>
       </c>
@@ -3006,7 +3001,7 @@
         <v>45935</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="15" customHeight="1">
+    <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>82</v>
       </c>
@@ -3017,7 +3012,7 @@
         <v>45935</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="15" customHeight="1">
+    <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>83</v>
       </c>
@@ -3028,7 +3023,7 @@
         <v>45939</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="15" customHeight="1">
+    <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>84</v>
       </c>
@@ -3039,7 +3034,7 @@
         <v>45939</v>
       </c>
     </row>
-    <row r="72" spans="2:6" ht="15" customHeight="1">
+    <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>85</v>
       </c>
@@ -3050,7 +3045,7 @@
         <v>45944</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="15" customHeight="1">
+    <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="22" t="s">
         <v>86</v>
       </c>
@@ -3061,7 +3056,7 @@
         <v>45944</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="15" customHeight="1">
+    <row r="74" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>87</v>
       </c>
@@ -3072,7 +3067,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="15" customHeight="1">
+    <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="22" t="s">
         <v>88</v>
       </c>
@@ -3083,7 +3078,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="15" customHeight="1">
+    <row r="76" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="22" t="s">
         <v>89</v>
       </c>
@@ -3094,7 +3089,7 @@
         <v>45946</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="15" customHeight="1">
+    <row r="77" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="22" t="s">
         <v>90</v>
       </c>
@@ -3105,7 +3100,7 @@
         <v>45946</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="15" customHeight="1">
+    <row r="78" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="22" t="s">
         <v>91</v>
       </c>
@@ -3116,7 +3111,7 @@
         <v>45946</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="15" customHeight="1">
+    <row r="79" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>92</v>
       </c>
@@ -3127,7 +3122,7 @@
         <v>45946</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="15" customHeight="1">
+    <row r="80" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>93</v>
       </c>
@@ -3138,7 +3133,7 @@
         <v>45946</v>
       </c>
     </row>
-    <row r="81" spans="2:6" ht="15" customHeight="1">
+    <row r="81" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>94</v>
       </c>
@@ -3149,7 +3144,7 @@
         <v>45949</v>
       </c>
     </row>
-    <row r="82" spans="2:6" ht="15" customHeight="1">
+    <row r="82" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>95</v>
       </c>
@@ -3163,7 +3158,7 @@
         <v>45952</v>
       </c>
     </row>
-    <row r="83" spans="2:6" ht="15" customHeight="1">
+    <row r="83" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>96</v>
       </c>
@@ -3174,7 +3169,7 @@
         <v>45949</v>
       </c>
     </row>
-    <row r="84" spans="2:6" ht="15" customHeight="1">
+    <row r="84" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>97</v>
       </c>
@@ -3185,7 +3180,7 @@
         <v>45950</v>
       </c>
     </row>
-    <row r="85" spans="2:6" ht="15" customHeight="1">
+    <row r="85" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>98</v>
       </c>
@@ -3193,7 +3188,7 @@
         <v>45950</v>
       </c>
     </row>
-    <row r="86" spans="2:6" ht="15" customHeight="1">
+    <row r="86" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>99</v>
       </c>
@@ -3201,7 +3196,7 @@
         <v>45950</v>
       </c>
     </row>
-    <row r="87" spans="2:6" ht="15" customHeight="1">
+    <row r="87" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>100</v>
       </c>
@@ -3212,7 +3207,7 @@
         <v>45950</v>
       </c>
     </row>
-    <row r="88" spans="2:6" ht="15" customHeight="1">
+    <row r="88" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>101</v>
       </c>
@@ -3223,7 +3218,7 @@
         <v>45950</v>
       </c>
     </row>
-    <row r="89" spans="2:6" ht="15" customHeight="1">
+    <row r="89" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>102</v>
       </c>
@@ -3234,7 +3229,7 @@
         <v>45951</v>
       </c>
     </row>
-    <row r="90" spans="2:6" ht="15" customHeight="1">
+    <row r="90" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>103</v>
       </c>
@@ -3242,7 +3237,7 @@
         <v>45953</v>
       </c>
     </row>
-    <row r="91" spans="2:6" ht="15" customHeight="1">
+    <row r="91" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>104</v>
       </c>
@@ -3254,7 +3249,7 @@
         <v>45953</v>
       </c>
     </row>
-    <row r="92" spans="2:6" ht="15" customHeight="1">
+    <row r="92" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>105</v>
       </c>
@@ -3262,7 +3257,7 @@
         <v>45953</v>
       </c>
     </row>
-    <row r="93" spans="2:6" ht="15" customHeight="1">
+    <row r="93" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>106</v>
       </c>
@@ -3270,7 +3265,7 @@
         <v>45953</v>
       </c>
     </row>
-    <row r="94" spans="2:6" ht="15" customHeight="1">
+    <row r="94" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>107</v>
       </c>
@@ -3278,7 +3273,7 @@
         <v>45953</v>
       </c>
     </row>
-    <row r="95" spans="2:6" ht="15" customHeight="1">
+    <row r="95" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>108</v>
       </c>
@@ -3289,17 +3284,17 @@
         <v>45957</v>
       </c>
     </row>
-    <row r="96" spans="2:6" ht="15" customHeight="1">
+    <row r="96" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="97" spans="2:6" ht="15" customHeight="1">
+    <row r="97" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="98" spans="2:6" ht="15" customHeight="1">
+    <row r="98" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>110</v>
       </c>
@@ -3310,7 +3305,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="99" spans="2:6" ht="15" customHeight="1">
+    <row r="99" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>111</v>
       </c>
@@ -3318,7 +3313,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="100" spans="2:6" ht="15" customHeight="1">
+    <row r="100" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>112</v>
       </c>
@@ -3329,7 +3324,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="101" spans="2:6" ht="15" customHeight="1">
+    <row r="101" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>113</v>
       </c>
@@ -3337,7 +3332,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="102" spans="2:6" ht="15" customHeight="1">
+    <row r="102" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>114</v>
       </c>
@@ -3345,7 +3340,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="103" spans="2:6" ht="15" customHeight="1">
+    <row r="103" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>115</v>
       </c>
@@ -3356,7 +3351,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="104" spans="2:6" ht="15" customHeight="1">
+    <row r="104" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>116</v>
       </c>
@@ -3367,7 +3362,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="105" spans="2:6" ht="15" customHeight="1">
+    <row r="105" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>117</v>
       </c>
@@ -3375,7 +3370,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="106" spans="2:6" ht="15" customHeight="1">
+    <row r="106" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>118</v>
       </c>
@@ -3383,7 +3378,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="107" spans="2:6" ht="15" customHeight="1">
+    <row r="107" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>119</v>
       </c>
@@ -3394,7 +3389,7 @@
         <v>45958</v>
       </c>
     </row>
-    <row r="108" spans="2:6" ht="15" customHeight="1">
+    <row r="108" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>120</v>
       </c>
@@ -3405,7 +3400,7 @@
         <v>45958</v>
       </c>
     </row>
-    <row r="109" spans="2:6" ht="15" customHeight="1">
+    <row r="109" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>121</v>
       </c>
@@ -3413,7 +3408,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="110" spans="2:6" ht="15" customHeight="1">
+    <row r="110" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>122</v>
       </c>
@@ -3421,7 +3416,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="111" spans="2:6" ht="15" customHeight="1">
+    <row r="111" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>123</v>
       </c>
@@ -3432,7 +3427,7 @@
         <v>45959</v>
       </c>
     </row>
-    <row r="112" spans="2:6" ht="15" customHeight="1">
+    <row r="112" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>124</v>
       </c>
@@ -3460,26 +3455,26 @@
       <selection activeCell="K105" sqref="K105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="14" width="21" customWidth="1"/>
-    <col min="15" max="17" width="21.140625" customWidth="1"/>
-    <col min="18" max="18" width="20.5703125" customWidth="1"/>
-    <col min="19" max="19" width="21.28515625" customWidth="1"/>
+    <col min="15" max="17" width="21.109375" customWidth="1"/>
+    <col min="18" max="18" width="20.5546875" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" customWidth="1"/>
     <col min="20" max="20" width="22" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" customWidth="1"/>
-    <col min="22" max="22" width="16.85546875" customWidth="1"/>
-    <col min="23" max="23" width="17.7109375" customWidth="1"/>
-    <col min="24" max="24" width="14.42578125" customWidth="1"/>
-    <col min="25" max="25" width="14.7109375" customWidth="1"/>
-    <col min="26" max="26" width="22.7109375" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" customWidth="1"/>
-    <col min="28" max="28" width="16.28515625" customWidth="1"/>
+    <col min="21" max="21" width="16.109375" customWidth="1"/>
+    <col min="22" max="22" width="16.88671875" customWidth="1"/>
+    <col min="23" max="23" width="17.6640625" customWidth="1"/>
+    <col min="24" max="24" width="14.44140625" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" customWidth="1"/>
+    <col min="26" max="26" width="22.6640625" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" customWidth="1"/>
+    <col min="28" max="28" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3565,7 +3560,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="13" customFormat="1" ht="15.6" customHeight="1">
+    <row r="2" spans="1:29" s="13" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1018</v>
       </c>
@@ -3616,7 +3611,7 @@
       <c r="AB2" s="18"/>
       <c r="AC2" s="17"/>
     </row>
-    <row r="3" spans="1:29" s="2" customFormat="1" ht="14.25" customHeight="1">
+    <row r="3" spans="1:29" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1019</v>
       </c>
@@ -3642,7 +3637,7 @@
       <c r="L3" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="M3" s="24">
+      <c r="M3" s="23">
         <v>45969</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -3664,7 +3659,7 @@
       <c r="AB3" s="5"/>
       <c r="AC3" s="4"/>
     </row>
-    <row r="4" spans="1:29" s="13" customFormat="1" ht="15.75" customHeight="1">
+    <row r="4" spans="1:29" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>1020</v>
       </c>
@@ -3708,7 +3703,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="13" customFormat="1">
+    <row r="5" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>1021</v>
       </c>
@@ -3750,7 +3745,7 @@
       <c r="AB5" s="18"/>
       <c r="AC5" s="17"/>
     </row>
-    <row r="6" spans="1:29" s="2" customFormat="1" ht="27.75" customHeight="1">
+    <row r="6" spans="1:29" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1022</v>
       </c>
@@ -3783,7 +3778,7 @@
       <c r="AB6" s="5"/>
       <c r="AC6" s="4"/>
     </row>
-    <row r="7" spans="1:29" s="9" customFormat="1" ht="18" customHeight="1">
+    <row r="7" spans="1:29" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>1024</v>
       </c>
@@ -3822,7 +3817,7 @@
       <c r="AB7" s="12"/>
       <c r="AC7" s="10"/>
     </row>
-    <row r="8" spans="1:29" s="2" customFormat="1" ht="14.25" customHeight="1">
+    <row r="8" spans="1:29" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1025</v>
       </c>
@@ -3851,7 +3846,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="9" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:29" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>1026</v>
       </c>
@@ -3877,7 +3872,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="13" customFormat="1">
+    <row r="10" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>1027</v>
       </c>
@@ -3904,33 +3899,33 @@
       <c r="AA10" s="18"/>
       <c r="AB10" s="18"/>
     </row>
-    <row r="11" spans="1:29" s="30" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A11" s="30">
+    <row r="11" spans="1:29" s="26" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26">
         <v>2002</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J11" s="28">
         <v>531471057</v>
       </c>
-      <c r="Y11" s="31" t="s">
+      <c r="Y11" s="27" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:29" s="13" customFormat="1" ht="30.75">
+    <row r="12" spans="1:29" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>2003</v>
       </c>
@@ -3956,7 +3951,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:29" s="13" customFormat="1">
+    <row r="13" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>2005</v>
       </c>
@@ -3977,7 +3972,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:29" s="13" customFormat="1">
+    <row r="14" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>198</v>
       </c>
@@ -4000,7 +3995,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:29" s="2" customFormat="1" ht="30.75">
+    <row r="15" spans="1:29" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>2007</v>
       </c>
@@ -4026,7 +4021,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="9" customFormat="1">
+    <row r="16" spans="1:29" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>2008</v>
       </c>
@@ -4046,7 +4041,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="9" customFormat="1">
+    <row r="17" spans="1:29" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>2009</v>
       </c>
@@ -4072,30 +4067,30 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="30" customFormat="1">
-      <c r="A18" s="30">
+    <row r="18" spans="1:29" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="26">
         <v>2010</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="J18" s="32">
+      <c r="J18" s="28">
         <v>503001412</v>
       </c>
-      <c r="Y18" s="31" t="s">
+      <c r="Y18" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="9" customFormat="1">
+    <row r="19" spans="1:29" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>2011</v>
       </c>
@@ -4124,7 +4119,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="21" customFormat="1">
+    <row r="20" spans="1:29" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2012</v>
       </c>
@@ -4167,7 +4162,7 @@
       <c r="AB20"/>
       <c r="AC20"/>
     </row>
-    <row r="21" spans="1:29" s="21" customFormat="1">
+    <row r="21" spans="1:29" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2013</v>
       </c>
@@ -4216,7 +4211,7 @@
       <c r="AB21"/>
       <c r="AC21"/>
     </row>
-    <row r="22" spans="1:29" s="21" customFormat="1">
+    <row r="22" spans="1:29" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2014</v>
       </c>
@@ -4257,7 +4252,7 @@
       <c r="AB22"/>
       <c r="AC22"/>
     </row>
-    <row r="23" spans="1:29" s="21" customFormat="1">
+    <row r="23" spans="1:29" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2015</v>
       </c>
@@ -4292,7 +4287,7 @@
       <c r="AB23"/>
       <c r="AC23"/>
     </row>
-    <row r="24" spans="1:29" s="13" customFormat="1">
+    <row r="24" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>2031</v>
       </c>
@@ -4315,7 +4310,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="13" customFormat="1">
+    <row r="25" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>2033</v>
       </c>
@@ -4335,7 +4330,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:29" s="13" customFormat="1">
+    <row r="26" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>2035</v>
       </c>
@@ -4358,7 +4353,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="13" customFormat="1" ht="30.75">
+    <row r="27" spans="1:29" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>2036</v>
       </c>
@@ -4381,7 +4376,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="13" customFormat="1" ht="30.75">
+    <row r="28" spans="1:29" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>2037</v>
       </c>
@@ -4407,7 +4402,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:29" s="13" customFormat="1" ht="30.75">
+    <row r="29" spans="1:29" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>2032</v>
       </c>
@@ -4430,7 +4425,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="30" spans="1:29" s="2" customFormat="1" ht="30.75">
+    <row r="30" spans="1:29" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>2038</v>
       </c>
@@ -4453,7 +4448,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="13" customFormat="1" ht="30.75">
+    <row r="31" spans="1:29" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>2039</v>
       </c>
@@ -4476,7 +4471,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="2" customFormat="1">
+    <row r="32" spans="1:29" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>2040</v>
       </c>
@@ -4496,7 +4491,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:25" s="13" customFormat="1">
+    <row r="33" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>2041</v>
       </c>
@@ -4516,7 +4511,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:25" s="13" customFormat="1" ht="30.75">
+    <row r="34" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>2042</v>
       </c>
@@ -4539,7 +4534,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="35" spans="1:25" s="2" customFormat="1" ht="30.75">
+    <row r="35" spans="1:25" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>2043</v>
       </c>
@@ -4565,7 +4560,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="13" customFormat="1" ht="30.75">
+    <row r="36" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>2044</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="2" customFormat="1" ht="30.75">
+    <row r="37" spans="1:25" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>242</v>
       </c>
@@ -4614,7 +4609,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="13" customFormat="1" ht="30.75">
+    <row r="38" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>2046</v>
       </c>
@@ -4637,7 +4632,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="13" customFormat="1">
+    <row r="39" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>2047</v>
       </c>
@@ -4660,7 +4655,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:25" s="13" customFormat="1" ht="45.75">
+    <row r="40" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>2048</v>
       </c>
@@ -4683,7 +4678,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:25" s="13" customFormat="1" ht="45.75">
+    <row r="41" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>2049</v>
       </c>
@@ -4706,7 +4701,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:25" s="13" customFormat="1" ht="30.75">
+    <row r="42" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="13">
         <v>2050</v>
       </c>
@@ -4729,7 +4724,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="43" spans="1:25" s="13" customFormat="1" ht="45.75">
+    <row r="43" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>2051</v>
       </c>
@@ -4755,7 +4750,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="13" customFormat="1" ht="30.75">
+    <row r="44" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>2052</v>
       </c>
@@ -4781,7 +4776,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="2" customFormat="1">
+    <row r="45" spans="1:25" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>2053</v>
       </c>
@@ -4807,7 +4802,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:25" s="13" customFormat="1">
+    <row r="46" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>2054</v>
       </c>
@@ -4827,7 +4822,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="47" spans="1:25" s="13" customFormat="1">
+    <row r="47" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>2055</v>
       </c>
@@ -4853,7 +4848,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="48" spans="1:25" s="13" customFormat="1" ht="30.75">
+    <row r="48" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>2056</v>
       </c>
@@ -4879,7 +4874,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:25" s="13" customFormat="1" ht="30.75">
+    <row r="49" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>2057</v>
       </c>
@@ -4902,7 +4897,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="13" customFormat="1" ht="45.75">
+    <row r="50" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>2058</v>
       </c>
@@ -4928,7 +4923,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="13" customFormat="1" ht="33.75" customHeight="1">
+    <row r="51" spans="1:25" s="13" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>2059</v>
       </c>
@@ -4954,7 +4949,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="1:25" s="13" customFormat="1" ht="45.75">
+    <row r="52" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
         <v>2060</v>
       </c>
@@ -4974,7 +4969,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="13" customFormat="1">
+    <row r="53" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>2061</v>
       </c>
@@ -4994,7 +4989,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="54" spans="1:25" s="13" customFormat="1" ht="45.75">
+    <row r="54" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="13">
         <v>2062</v>
       </c>
@@ -5020,7 +5015,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:25" s="2" customFormat="1" ht="30.75">
+    <row r="55" spans="1:25" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>2063</v>
       </c>
@@ -5043,7 +5038,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="1:25" s="13" customFormat="1">
+    <row r="56" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="13">
         <v>2064</v>
       </c>
@@ -5066,7 +5061,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="57" spans="1:25" s="13" customFormat="1" ht="45.75">
+    <row r="57" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="13">
         <v>2065</v>
       </c>
@@ -5092,7 +5087,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:25" s="13" customFormat="1" ht="45.75">
+    <row r="58" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="13">
         <v>2066</v>
       </c>
@@ -5118,7 +5113,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:25" s="13" customFormat="1" ht="45.75">
+    <row r="59" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="13">
         <v>2067</v>
       </c>
@@ -5141,7 +5136,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:25" s="13" customFormat="1" ht="30.75">
+    <row r="60" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="13">
         <v>2068</v>
       </c>
@@ -5167,7 +5162,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="61" spans="1:25" s="2" customFormat="1" ht="30.75">
+    <row r="61" spans="1:25" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>2069</v>
       </c>
@@ -5185,7 +5180,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="62" spans="1:25" s="13" customFormat="1">
+    <row r="62" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D62" s="16" t="s">
         <v>273</v>
       </c>
@@ -5202,7 +5197,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:25" s="13" customFormat="1">
+    <row r="63" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D63" s="13" t="s">
         <v>152</v>
       </c>
@@ -5219,7 +5214,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:25" s="13" customFormat="1" ht="30.75">
+    <row r="64" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D64" s="16" t="s">
         <v>273</v>
       </c>
@@ -5236,7 +5231,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="65" spans="4:28" s="13" customFormat="1" ht="15" customHeight="1">
+    <row r="65" spans="4:25" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D65" s="13" t="s">
         <v>152</v>
       </c>
@@ -5253,7 +5248,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="66" spans="4:28" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="66" spans="4:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D66" s="2" t="s">
         <v>200</v>
       </c>
@@ -5273,7 +5268,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="67" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="67" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D67" s="9" t="s">
         <v>183</v>
       </c>
@@ -5293,7 +5288,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="68" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D68" s="11" t="s">
         <v>283</v>
       </c>
@@ -5313,7 +5308,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="69" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="69" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D69" s="9" t="s">
         <v>285</v>
       </c>
@@ -5326,14 +5321,14 @@
       <c r="G69" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="K69" s="27" t="s">
+      <c r="K69" s="24" t="s">
         <v>287</v>
       </c>
       <c r="Y69" s="9" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="70" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="70" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D70" s="11" t="s">
         <v>288</v>
       </c>
@@ -5353,27 +5348,27 @@
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="4:28" s="26" customFormat="1" ht="15" customHeight="1">
-      <c r="D71" s="26" t="s">
+    <row r="71" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
         <v>183</v>
       </c>
-      <c r="E71" s="26" t="s">
+      <c r="E71" t="s">
         <v>84</v>
       </c>
-      <c r="F71" s="26" t="s">
+      <c r="F71" t="s">
         <v>261</v>
       </c>
-      <c r="G71" s="26" t="s">
+      <c r="G71" t="s">
         <v>193</v>
       </c>
-      <c r="J71" s="26">
+      <c r="J71">
         <v>591177100</v>
       </c>
-      <c r="Y71" s="26" t="s">
+      <c r="Y71" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="72" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D72" s="9" t="s">
         <v>183</v>
       </c>
@@ -5393,7 +5388,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="73" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D73" s="9" t="s">
         <v>285</v>
       </c>
@@ -5410,7 +5405,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="74" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="74" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D74" s="9" t="s">
         <v>183</v>
       </c>
@@ -5430,7 +5425,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="75" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="75" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D75" s="9" t="s">
         <v>183</v>
       </c>
@@ -5450,7 +5445,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="76" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="76" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D76" s="9" t="s">
         <v>294</v>
       </c>
@@ -5467,7 +5462,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="77" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="77" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D77" s="9" t="s">
         <v>183</v>
       </c>
@@ -5489,10 +5484,8 @@
       <c r="Y77" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="AA77" s="25"/>
-      <c r="AB77" s="25"/>
-    </row>
-    <row r="78" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="78" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D78" s="9" t="s">
         <v>296</v>
       </c>
@@ -5514,10 +5507,8 @@
       <c r="Y78" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="AA78" s="25"/>
-      <c r="AB78" s="25"/>
-    </row>
-    <row r="79" spans="4:28" s="9" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="79" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D79" s="9" t="s">
         <v>183</v>
       </c>
@@ -5536,10 +5527,8 @@
       <c r="Y79" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="AA79" s="25"/>
-      <c r="AB79" s="25"/>
-    </row>
-    <row r="80" spans="4:28" s="9" customFormat="1">
+    </row>
+    <row r="80" spans="4:25" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D80" s="9" t="s">
         <v>183</v>
       </c>
@@ -5555,39 +5544,35 @@
       <c r="J80" s="9">
         <v>556369447</v>
       </c>
-      <c r="Y80" s="25" t="s">
+      <c r="Y80" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="AA80" s="25"/>
-      <c r="AB80" s="25"/>
-    </row>
-    <row r="81" spans="4:28" s="30" customFormat="1" ht="15" customHeight="1">
-      <c r="D81" s="30" t="s">
+    </row>
+    <row r="81" spans="4:25" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D81" s="26" t="s">
         <v>273</v>
       </c>
-      <c r="E81" s="30" t="s">
+      <c r="E81" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F81" s="30" t="s">
+      <c r="F81" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="G81" s="30" t="s">
+      <c r="G81" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="I81" s="30" t="s">
+      <c r="I81" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="J81" s="30">
+      <c r="J81" s="26">
         <v>549228994</v>
       </c>
-      <c r="Y81" s="33">
-        <f ca="1">A80:Y101</f>
+      <c r="Y81" s="26">
+        <f t="shared" ref="Y81:Y94" ca="1" si="0">A80:Y101</f>
         <v>0</v>
       </c>
-      <c r="AA81" s="33"/>
-      <c r="AB81" s="33"/>
-    </row>
-    <row r="82" spans="4:28" ht="15" customHeight="1">
+    </row>
+    <row r="82" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
         <v>304</v>
       </c>
@@ -5603,14 +5588,12 @@
       <c r="J82">
         <v>500192554</v>
       </c>
-      <c r="Y82" s="23">
-        <f ca="1">A81:Y102</f>
+      <c r="Y82">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA82" s="23"/>
-      <c r="AB82" s="23"/>
-    </row>
-    <row r="83" spans="4:28" ht="15" customHeight="1">
+    </row>
+    <row r="83" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D83" t="s">
         <v>251</v>
       </c>
@@ -5629,14 +5612,12 @@
       <c r="J83">
         <v>503880000</v>
       </c>
-      <c r="Y83" s="23">
-        <f ca="1">A82:Y103</f>
+      <c r="Y83">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA83" s="23"/>
-      <c r="AB83" s="23"/>
-    </row>
-    <row r="84" spans="4:28" s="13" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="84" spans="4:25" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D84" s="13" t="s">
         <v>273</v>
       </c>
@@ -5655,14 +5636,12 @@
       <c r="J84" s="13">
         <v>554949955</v>
       </c>
-      <c r="Y84" s="28">
-        <f ca="1">A83:Y104</f>
+      <c r="Y84" s="13">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA84" s="28"/>
-      <c r="AB84" s="28"/>
-    </row>
-    <row r="85" spans="4:28" ht="15" customHeight="1">
+    </row>
+    <row r="85" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
         <v>308</v>
       </c>
@@ -5681,14 +5660,12 @@
       <c r="J85">
         <v>506399464</v>
       </c>
-      <c r="Y85" s="23">
-        <f ca="1">A84:Y105</f>
+      <c r="Y85">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA85" s="23"/>
-      <c r="AB85" s="23"/>
-    </row>
-    <row r="86" spans="4:28" ht="15" customHeight="1">
+    </row>
+    <row r="86" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
         <v>190</v>
       </c>
@@ -5698,63 +5675,57 @@
       <c r="G86" t="s">
         <v>154</v>
       </c>
-      <c r="Y86" s="23">
-        <f ca="1">A85:Y106</f>
+      <c r="Y86">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA86" s="23"/>
-      <c r="AB86" s="23"/>
-    </row>
-    <row r="87" spans="4:28" s="30" customFormat="1" ht="15" customHeight="1">
-      <c r="D87" s="30" t="s">
+    </row>
+    <row r="87" spans="4:25" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D87" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="E87" s="30" t="s">
+      <c r="E87" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="F87" s="30" t="s">
+      <c r="F87" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="G87" s="30" t="s">
+      <c r="G87" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="I87" s="30" t="s">
+      <c r="I87" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="J87" s="30">
+      <c r="J87" s="26">
         <v>557652698</v>
       </c>
-      <c r="Y87" s="33">
-        <f ca="1">A86:Y107</f>
+      <c r="Y87" s="26">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA87" s="33"/>
-      <c r="AB87" s="33"/>
-    </row>
-    <row r="88" spans="4:28" s="30" customFormat="1" ht="15" customHeight="1">
-      <c r="D88" s="30" t="s">
+    </row>
+    <row r="88" spans="4:25" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D88" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="E88" s="30" t="s">
+      <c r="E88" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="F88" s="30" t="s">
+      <c r="F88" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="I88" s="30" t="s">
+      <c r="I88" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="J88" s="30">
+      <c r="J88" s="26">
         <v>581930093</v>
       </c>
-      <c r="Y88" s="33">
-        <f ca="1">A87:Y108</f>
+      <c r="Y88" s="26">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA88" s="33"/>
-      <c r="AB88" s="33"/>
-    </row>
-    <row r="89" spans="4:28" ht="15" customHeight="1">
+    </row>
+    <row r="89" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
         <v>183</v>
       </c>
@@ -5770,116 +5741,102 @@
       <c r="J89">
         <v>563310927</v>
       </c>
-      <c r="Y89" s="23">
-        <f ca="1">A88:Y109</f>
+      <c r="Y89">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA89" s="23"/>
-      <c r="AB89" s="23"/>
-    </row>
-    <row r="90" spans="4:28" s="30" customFormat="1" ht="15" customHeight="1">
-      <c r="D90" s="30" t="s">
+    </row>
+    <row r="90" spans="4:25" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D90" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="E90" s="30" t="s">
+      <c r="E90" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="Y90" s="33">
-        <f ca="1">A89:Y110</f>
+      <c r="Y90" s="26">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA90" s="33"/>
-      <c r="AB90" s="33"/>
-    </row>
-    <row r="91" spans="4:28" s="30" customFormat="1" ht="15" customHeight="1">
-      <c r="D91" s="30" t="s">
+    </row>
+    <row r="91" spans="4:25" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D91" s="26" t="s">
         <v>318</v>
       </c>
-      <c r="E91" s="30" t="s">
+      <c r="E91" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="F91" s="30" t="s">
+      <c r="F91" s="26" t="s">
         <v>319</v>
       </c>
-      <c r="I91" s="30" t="s">
+      <c r="I91" s="26" t="s">
         <v>320</v>
       </c>
-      <c r="J91" s="30">
+      <c r="J91" s="26">
         <v>554000208</v>
       </c>
-      <c r="Y91" s="33">
-        <f ca="1">A90:Y111</f>
+      <c r="Y91" s="26">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA91" s="33"/>
-      <c r="AB91" s="33"/>
-    </row>
-    <row r="92" spans="4:28" s="30" customFormat="1" ht="15" customHeight="1">
-      <c r="D92" s="30" t="s">
+    </row>
+    <row r="92" spans="4:25" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D92" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="E92" s="30" t="s">
+      <c r="E92" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="Y92" s="33">
-        <f ca="1">A91:Y112</f>
+      <c r="Y92" s="26">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA92" s="33"/>
-      <c r="AB92" s="33"/>
-    </row>
-    <row r="93" spans="4:28" s="30" customFormat="1" ht="15" customHeight="1">
-      <c r="D93" s="30" t="s">
+    </row>
+    <row r="93" spans="4:25" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D93" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="E93" s="30" t="s">
+      <c r="E93" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="Y93" s="33">
-        <f ca="1">A92:Y113</f>
+      <c r="Y93" s="26">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA93" s="33"/>
-      <c r="AB93" s="33"/>
-    </row>
-    <row r="94" spans="4:28" s="30" customFormat="1" ht="15" customHeight="1">
-      <c r="D94" s="30" t="s">
+    </row>
+    <row r="94" spans="4:25" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D94" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="E94" s="30" t="s">
+      <c r="E94" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="Y94" s="33">
-        <f ca="1">A93:Y114</f>
+      <c r="Y94" s="26">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA94" s="33"/>
-      <c r="AB94" s="33"/>
-    </row>
-    <row r="95" spans="4:28" s="30" customFormat="1" ht="15" customHeight="1">
-      <c r="D95" s="30" t="s">
+    </row>
+    <row r="95" spans="4:25" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D95" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="E95" s="30" t="s">
+      <c r="E95" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="F95" s="30" t="s">
+      <c r="F95" s="26" t="s">
         <v>322</v>
       </c>
-      <c r="I95" s="30" t="s">
+      <c r="I95" s="26" t="s">
         <v>320</v>
       </c>
-      <c r="J95" s="30">
+      <c r="J95" s="26">
         <v>580220982</v>
       </c>
-      <c r="Y95" s="33">
+      <c r="Y95" s="26">
         <f ca="1">A94:Y143</f>
         <v>0</v>
       </c>
-      <c r="AA95" s="33"/>
-      <c r="AB95" s="33"/>
-    </row>
-    <row r="96" spans="4:28" ht="15" customHeight="1">
+    </row>
+    <row r="96" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E96" t="s">
         <v>109</v>
       </c>
@@ -5895,14 +5852,12 @@
       <c r="J96">
         <v>545669065</v>
       </c>
-      <c r="Y96" s="23">
+      <c r="Y96">
         <f ca="1">A95:Y116</f>
         <v>0</v>
       </c>
-      <c r="AA96" s="23"/>
-      <c r="AB96" s="23"/>
-    </row>
-    <row r="97" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="97" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E97" t="s">
         <v>89</v>
       </c>
@@ -5918,14 +5873,12 @@
       <c r="J97">
         <v>595020128</v>
       </c>
-      <c r="Y97" s="23">
+      <c r="Y97">
         <f ca="1">A97:Y118</f>
         <v>0</v>
       </c>
-      <c r="AA97" s="23"/>
-      <c r="AB97" s="23"/>
-    </row>
-    <row r="98" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="98" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D98" t="s">
         <v>251</v>
       </c>
@@ -5941,14 +5894,12 @@
       <c r="J98">
         <v>541155533</v>
       </c>
-      <c r="Y98" s="23">
-        <f ca="1">A97:Y118</f>
+      <c r="Y98">
+        <f t="shared" ref="Y98:Y115" ca="1" si="1">A97:Y118</f>
         <v>0</v>
       </c>
-      <c r="AA98" s="23"/>
-      <c r="AB98" s="23"/>
-    </row>
-    <row r="99" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="99" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D99" t="s">
         <v>183</v>
       </c>
@@ -5964,14 +5915,12 @@
       <c r="J99">
         <v>506503636</v>
       </c>
-      <c r="Y99" s="23">
-        <f ca="1">A98:Y119</f>
+      <c r="Y99">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA99" s="23"/>
-      <c r="AB99" s="23"/>
-    </row>
-    <row r="100" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="100" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D100" t="s">
         <v>251</v>
       </c>
@@ -5987,14 +5936,12 @@
       <c r="J100">
         <v>593777790</v>
       </c>
-      <c r="Y100" s="23">
-        <f ca="1">A99:Y120</f>
+      <c r="Y100">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA100" s="23"/>
-      <c r="AB100" s="23"/>
-    </row>
-    <row r="101" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="101" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D101" t="s">
         <v>183</v>
       </c>
@@ -6010,28 +5957,24 @@
       <c r="J101">
         <v>556622716</v>
       </c>
-      <c r="Y101" s="23">
-        <f ca="1">A100:Y121</f>
+      <c r="Y101">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA101" s="23"/>
-      <c r="AB101" s="23"/>
-    </row>
-    <row r="102" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="102" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D102" t="s">
         <v>190</v>
       </c>
       <c r="E102" t="s">
         <v>114</v>
       </c>
-      <c r="Y102" s="23">
-        <f ca="1">A101:Y122</f>
+      <c r="Y102">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA102" s="23"/>
-      <c r="AB102" s="23"/>
-    </row>
-    <row r="103" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="103" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D103" t="s">
         <v>332</v>
       </c>
@@ -6047,14 +5990,12 @@
       <c r="J103">
         <v>534859217</v>
       </c>
-      <c r="Y103" s="23">
-        <f ca="1">A102:Y123</f>
+      <c r="Y103">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA103" s="23"/>
-      <c r="AB103" s="23"/>
-    </row>
-    <row r="104" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="104" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D104" t="s">
         <v>334</v>
       </c>
@@ -6070,17 +6011,15 @@
       <c r="J104">
         <v>592482486</v>
       </c>
-      <c r="K104" s="29" t="s">
+      <c r="K104" s="25" t="s">
         <v>337</v>
       </c>
-      <c r="Y104" s="23">
-        <f ca="1">A103:Y124</f>
+      <c r="Y104">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA104" s="23"/>
-      <c r="AB104" s="23"/>
-    </row>
-    <row r="105" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="105" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D105" t="s">
         <v>183</v>
       </c>
@@ -6096,14 +6035,12 @@
       <c r="J105">
         <v>506486949</v>
       </c>
-      <c r="Y105" s="23">
-        <f ca="1">A104:Y125</f>
+      <c r="Y105">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA105" s="23"/>
-      <c r="AB105" s="23"/>
-    </row>
-    <row r="106" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="106" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D106" t="s">
         <v>183</v>
       </c>
@@ -6119,14 +6056,12 @@
       <c r="J106">
         <v>500800864</v>
       </c>
-      <c r="Y106" s="23">
-        <f ca="1">A105:Y126</f>
+      <c r="Y106">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA106" s="23"/>
-      <c r="AB106" s="23"/>
-    </row>
-    <row r="107" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="107" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>0</v>
       </c>
@@ -6145,14 +6080,12 @@
       <c r="J107">
         <v>508887437</v>
       </c>
-      <c r="Y107" s="23">
-        <f ca="1">A106:Y127</f>
+      <c r="Y107">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA107" s="23"/>
-      <c r="AB107" s="23"/>
-    </row>
-    <row r="108" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="108" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D108" t="s">
         <v>334</v>
       </c>
@@ -6168,17 +6101,15 @@
       <c r="J108">
         <v>560071794</v>
       </c>
-      <c r="K108" s="29" t="s">
+      <c r="K108" s="25" t="s">
         <v>344</v>
       </c>
-      <c r="Y108" s="23">
-        <f ca="1">A107:Y128</f>
+      <c r="Y108">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA108" s="23"/>
-      <c r="AB108" s="23"/>
-    </row>
-    <row r="109" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="109" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D109" t="s">
         <v>183</v>
       </c>
@@ -6194,14 +6125,12 @@
       <c r="J109">
         <v>504544073</v>
       </c>
-      <c r="Y109" s="23">
-        <f ca="1">A108:Y129</f>
+      <c r="Y109">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA109" s="23"/>
-      <c r="AB109" s="23"/>
-    </row>
-    <row r="110" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="110" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D110" t="s">
         <v>183</v>
       </c>
@@ -6217,14 +6146,12 @@
       <c r="J110">
         <v>503674125</v>
       </c>
-      <c r="Y110" s="23">
-        <f ca="1">A109:Y130</f>
+      <c r="Y110">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA110" s="23"/>
-      <c r="AB110" s="23"/>
-    </row>
-    <row r="111" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="111" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D111" t="s">
         <v>334</v>
       </c>
@@ -6240,17 +6167,15 @@
       <c r="J111">
         <v>561161461</v>
       </c>
-      <c r="K111" s="29" t="s">
+      <c r="K111" s="25" t="s">
         <v>351</v>
       </c>
-      <c r="Y111" s="23">
-        <f ca="1">A110:Y131</f>
+      <c r="Y111">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA111" s="23"/>
-      <c r="AB111" s="23"/>
-    </row>
-    <row r="112" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="112" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D112" t="s">
         <v>334</v>
       </c>
@@ -6266,257 +6191,195 @@
       <c r="J112">
         <v>500188766</v>
       </c>
-      <c r="K112" s="29" t="s">
+      <c r="K112" s="25" t="s">
         <v>354</v>
       </c>
-      <c r="Y112" s="23">
-        <f ca="1">A111:Y132</f>
+      <c r="Y112">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA112" s="23"/>
-      <c r="AB112" s="23"/>
-    </row>
-    <row r="113" spans="25:28" ht="15" customHeight="1">
-      <c r="Y113" s="23">
-        <f ca="1">A112:Y133</f>
+    </row>
+    <row r="113" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y113">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA113" s="23"/>
-      <c r="AB113" s="23"/>
-    </row>
-    <row r="114" spans="25:28" ht="15" customHeight="1">
-      <c r="Y114" s="23">
-        <f ca="1">A113:Y134</f>
+    </row>
+    <row r="114" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y114">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA114" s="23"/>
-      <c r="AB114" s="23"/>
-    </row>
-    <row r="115" spans="25:28" ht="15" customHeight="1">
-      <c r="Y115" s="23">
-        <f ca="1">A114:Y135</f>
+    </row>
+    <row r="115" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y115">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA115" s="23"/>
-      <c r="AB115" s="23"/>
-    </row>
-    <row r="116" spans="25:28" ht="15" customHeight="1">
-      <c r="Y116" s="23">
-        <f t="shared" ref="Y116:Y142" ca="1" si="0">A115:Y137</f>
+    </row>
+    <row r="116" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y116">
+        <f t="shared" ref="Y116:Y142" ca="1" si="2">A115:Y137</f>
         <v>0</v>
       </c>
-      <c r="AA116" s="23"/>
-      <c r="AB116" s="23"/>
-    </row>
-    <row r="117" spans="25:28" ht="15" customHeight="1">
-      <c r="Y117" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="117" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y117">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA117" s="23"/>
-      <c r="AB117" s="23"/>
-    </row>
-    <row r="118" spans="25:28" ht="15" customHeight="1">
-      <c r="Y118" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="118" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y118">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA118" s="23"/>
-      <c r="AB118" s="23"/>
-    </row>
-    <row r="119" spans="25:28" ht="15" customHeight="1">
-      <c r="Y119" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="119" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y119">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA119" s="23"/>
-      <c r="AB119" s="23"/>
-    </row>
-    <row r="120" spans="25:28" ht="15" customHeight="1">
-      <c r="Y120" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="120" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y120">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA120" s="23"/>
-      <c r="AB120" s="23"/>
-    </row>
-    <row r="121" spans="25:28" ht="15" customHeight="1">
-      <c r="Y121" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="121" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y121">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA121" s="23"/>
-      <c r="AB121" s="23"/>
-    </row>
-    <row r="122" spans="25:28" ht="15" customHeight="1">
-      <c r="Y122" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="122" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y122">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA122" s="23"/>
-      <c r="AB122" s="23"/>
-    </row>
-    <row r="123" spans="25:28" ht="15" customHeight="1">
-      <c r="Y123" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="123" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y123">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA123" s="23"/>
-      <c r="AB123" s="23"/>
-    </row>
-    <row r="124" spans="25:28" ht="15" customHeight="1">
-      <c r="Y124" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="124" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y124">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA124" s="23"/>
-      <c r="AB124" s="23"/>
-    </row>
-    <row r="125" spans="25:28" ht="15" customHeight="1">
-      <c r="Y125" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="125" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y125">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA125" s="23"/>
-      <c r="AB125" s="23"/>
-    </row>
-    <row r="126" spans="25:28" ht="15" customHeight="1">
-      <c r="Y126" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="126" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y126">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA126" s="23"/>
-      <c r="AB126" s="23"/>
-    </row>
-    <row r="127" spans="25:28" ht="15" customHeight="1">
-      <c r="Y127" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="127" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y127">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA127" s="23"/>
-      <c r="AB127" s="23"/>
-    </row>
-    <row r="128" spans="25:28" ht="15" customHeight="1">
-      <c r="Y128" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="128" spans="25:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y128">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA128" s="23"/>
-      <c r="AB128" s="23"/>
-    </row>
-    <row r="129" spans="1:28" ht="15" customHeight="1">
-      <c r="Y129" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="129" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y129">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA129" s="23"/>
-      <c r="AB129" s="23"/>
-    </row>
-    <row r="130" spans="1:28" ht="15" customHeight="1">
-      <c r="Y130" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="130" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y130">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA130" s="23"/>
-      <c r="AB130" s="23"/>
-    </row>
-    <row r="131" spans="1:28" ht="15" customHeight="1">
-      <c r="Y131" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="131" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y131">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA131" s="23"/>
-      <c r="AB131" s="23"/>
-    </row>
-    <row r="132" spans="1:28" ht="15" customHeight="1">
-      <c r="Y132" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="132" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y132">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA132" s="23"/>
-      <c r="AB132" s="23"/>
-    </row>
-    <row r="133" spans="1:28" ht="15" customHeight="1">
-      <c r="Y133" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="133" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y133">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA133" s="23"/>
-      <c r="AB133" s="23"/>
-    </row>
-    <row r="134" spans="1:28" ht="15" customHeight="1">
-      <c r="Y134" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="134" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y134">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA134" s="23"/>
-      <c r="AB134" s="23"/>
-    </row>
-    <row r="135" spans="1:28" ht="15" customHeight="1">
-      <c r="Y135" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="135" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y135">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA135" s="23"/>
-      <c r="AB135" s="23"/>
-    </row>
-    <row r="136" spans="1:28" ht="15" customHeight="1">
-      <c r="Y136" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="136" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y136">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA136" s="23"/>
-      <c r="AB136" s="23"/>
-    </row>
-    <row r="137" spans="1:28" ht="15" customHeight="1">
-      <c r="Y137" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="137" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y137">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA137" s="23"/>
-      <c r="AB137" s="23"/>
-    </row>
-    <row r="138" spans="1:28" ht="15" customHeight="1">
-      <c r="Y138" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="138" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y138">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA138" s="23"/>
-      <c r="AB138" s="23"/>
-    </row>
-    <row r="139" spans="1:28" ht="15" customHeight="1">
-      <c r="Y139" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="139" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y139">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA139" s="23"/>
-      <c r="AB139" s="23"/>
-    </row>
-    <row r="140" spans="1:28" ht="15" customHeight="1">
-      <c r="Y140" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="140" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y140">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA140" s="23"/>
-      <c r="AB140" s="23"/>
-    </row>
-    <row r="141" spans="1:28" ht="15" customHeight="1">
-      <c r="Y141" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="141" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y141">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA141" s="23"/>
-      <c r="AB141" s="23"/>
-    </row>
-    <row r="142" spans="1:28" ht="15" customHeight="1">
-      <c r="Y142" s="23">
-        <f t="shared" ca="1" si="0"/>
+    </row>
+    <row r="142" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y142">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA142" s="23"/>
-      <c r="AB142" s="23"/>
-    </row>
-    <row r="143" spans="1:28" ht="15" customHeight="1">
+    </row>
+    <row r="143" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>355</v>
       </c>
@@ -6562,15 +6425,15 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>356</v>
       </c>
@@ -6584,7 +6447,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>360</v>
       </c>
@@ -6598,7 +6461,7 @@
         <v>45939</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -6612,7 +6475,7 @@
         <v>45942</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G4">
         <v>62</v>
       </c>
@@ -6620,7 +6483,7 @@
         <v>45943</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G5">
         <v>67</v>
       </c>
@@ -6628,7 +6491,7 @@
         <v>45944</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G6">
         <v>59</v>
       </c>
@@ -6636,7 +6499,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G7">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Update khloud reports.xlsx with new data
</commit_message>
<xml_diff>
--- a/data/khloud reports.xlsx
+++ b/data/khloud reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1dc152c07513850c/Documents/GitHub/DataAnalyzer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1797" documentId="13_ncr:1_{400F4DCB-612B-46F1-BD96-90EED01F7942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB676D48-89F5-41F1-973A-7AFA95890FA9}"/>
+  <xr:revisionPtr revIDLastSave="1824" documentId="13_ncr:1_{400F4DCB-612B-46F1-BD96-90EED01F7942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{068EDA25-A333-4B5A-91C1-35D7BCAB92E7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="599" xr2:uid="{D0D76AE6-8D3C-4E35-ACCF-21D60420B679}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="357">
   <si>
     <t>Client serial number</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>Unilever Arabia (KSA ops)</t>
+  </si>
+  <si>
+    <t>Gulf Central Company</t>
   </si>
   <si>
     <t>Card creation date</t>
@@ -1087,9 +1090,6 @@
     <t>leen.alsulami@unilever.com</t>
   </si>
   <si>
-    <t>Gulf Central Company</t>
-  </si>
-  <si>
     <t>barakat</t>
   </si>
   <si>
@@ -1109,6 +1109,9 @@
   </si>
   <si>
     <t>saco</t>
+  </si>
+  <si>
+    <t>pioneers medical</t>
   </si>
 </sst>
 </file>
@@ -1871,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B1EC1C-85F6-4EA5-A96A-3DBA3CF0DE98}">
-  <dimension ref="A1:O108"/>
+  <dimension ref="A1:O109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="I98" sqref="I98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2458,6 +2461,9 @@
       <c r="G33" s="8">
         <v>45907</v>
       </c>
+      <c r="H33" s="8">
+        <v>45907</v>
+      </c>
     </row>
     <row r="34" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -3358,6 +3364,17 @@
       </c>
       <c r="E108" s="8">
         <v>45956</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>121</v>
+      </c>
+      <c r="E109" s="8">
+        <v>45960</v>
+      </c>
+      <c r="F109" s="8">
+        <v>45960</v>
       </c>
     </row>
   </sheetData>
@@ -3376,8 +3393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A124B1-A62D-41C1-80E4-6E6C588E4C8F}">
   <dimension ref="A1:AC140"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="H108" sqref="H108"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3405,85 +3422,85 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="P1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="W1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="X1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Y1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Z1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AA1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AB1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="13" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3491,48 +3508,48 @@
         <v>1018</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K2" s="14">
         <v>554599660</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N2" s="15">
         <v>45938</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="W2" s="16"/>
       <c r="X2" s="16"/>
       <c r="Y2" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="Z2" s="17"/>
       <c r="AA2" s="18"/>
@@ -3544,35 +3561,35 @@
         <v>1019</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N3" s="22">
         <v>45969</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
@@ -3580,10 +3597,10 @@
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
       <c r="V3" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Y3" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="Z3" s="4"/>
       <c r="AA3" s="5"/>
@@ -3595,46 +3612,46 @@
         <v>1020</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K4" s="14">
         <v>508011110</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="V4" s="13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Y4" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3642,40 +3659,40 @@
         <v>1021</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K5" s="14">
         <v>505225136</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="V5" s="13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Y5" s="13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Z5" s="17"/>
       <c r="AA5" s="18"/>
@@ -3687,31 +3704,31 @@
         <v>1022</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Y6" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Z6" s="4"/>
       <c r="AA6" s="5"/>
@@ -3723,37 +3740,37 @@
         <v>1024</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K7" s="19">
         <v>505903400</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="V7" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Z7" s="10"/>
       <c r="AA7" s="12"/>
@@ -3765,31 +3782,31 @@
         <v>1025</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K8" s="6">
         <v>535100774</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Y8" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:29" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3797,28 +3814,28 @@
         <v>1026</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K9" s="19">
         <v>504606130</v>
       </c>
       <c r="Y9" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3826,26 +3843,26 @@
         <v>1027</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K10" s="20"/>
       <c r="Y10" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="Z10" s="17"/>
       <c r="AA10" s="18"/>
@@ -3856,28 +3873,28 @@
         <v>2002</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K11" s="27">
         <v>531471057</v>
       </c>
       <c r="Y11" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:29" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3885,28 +3902,28 @@
         <v>2003</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K12" s="20">
         <v>558558331</v>
       </c>
       <c r="Y12" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3914,49 +3931,49 @@
         <v>2005</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K13" s="20"/>
       <c r="Y13" s="13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:29" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>27</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K14" s="20">
         <v>555810508</v>
       </c>
       <c r="Y14" s="13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:29" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3964,28 +3981,28 @@
         <v>2007</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K15" s="6">
         <v>537216154</v>
       </c>
       <c r="Y15" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:29" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3993,22 +4010,22 @@
         <v>2008</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K16" s="19">
         <v>597004024</v>
       </c>
       <c r="Y16" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:25" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4016,28 +4033,28 @@
         <v>2009</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K17" s="19">
         <v>551390000</v>
       </c>
       <c r="Y17" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:25" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4045,25 +4062,25 @@
         <v>2010</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>31</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K18" s="27">
         <v>503001412</v>
       </c>
       <c r="Y18" s="26" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:25" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4071,31 +4088,31 @@
         <v>2011</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="K19" s="19">
         <v>550855851</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="Y19" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4103,25 +4120,25 @@
         <v>2031</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K20" s="20">
         <v>500605918</v>
       </c>
       <c r="Y20" s="13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4129,22 +4146,22 @@
         <v>2033</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K21" s="20">
         <v>530016343</v>
       </c>
       <c r="Y21" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4152,25 +4169,25 @@
         <v>2035</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>35</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K22" s="20">
         <v>562720868</v>
       </c>
       <c r="Y22" s="13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4178,25 +4195,25 @@
         <v>2036</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>36</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K23" s="20">
         <v>551992419</v>
       </c>
       <c r="Y23" s="16" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4204,28 +4221,28 @@
         <v>2037</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>37</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K24" s="20">
         <v>533595536</v>
       </c>
       <c r="Y24" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4233,25 +4250,25 @@
         <v>2032</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K25" s="20">
         <v>503232092</v>
       </c>
       <c r="Y25" s="16" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:25" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4259,25 +4276,25 @@
         <v>2038</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K26" s="6">
         <v>545161853</v>
       </c>
       <c r="Y26" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4285,25 +4302,25 @@
         <v>2039</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>40</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K27" s="20">
         <v>562082902</v>
       </c>
       <c r="Y27" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:25" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4311,22 +4328,22 @@
         <v>2040</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K28" s="6">
         <v>557285215</v>
       </c>
       <c r="Y28" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4334,22 +4351,22 @@
         <v>2041</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>42</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K29" s="20">
         <v>570594590</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4357,25 +4374,25 @@
         <v>2042</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>43</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K30" s="20">
         <v>507672155</v>
       </c>
       <c r="Y30" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:25" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4383,28 +4400,28 @@
         <v>2043</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K31" s="6">
         <v>544293555</v>
       </c>
       <c r="Y31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4412,54 +4429,54 @@
         <v>2044</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>45</v>
       </c>
       <c r="F32" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="J32" s="13" t="s">
         <v>231</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>230</v>
       </c>
       <c r="K32" s="20">
         <v>564469119</v>
       </c>
       <c r="Y32" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:25" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K33" s="6">
         <v>580706157</v>
       </c>
       <c r="Y33" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4467,25 +4484,25 @@
         <v>2046</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>47</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K34" s="20">
         <v>559072756</v>
       </c>
       <c r="Y34" s="16" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4493,25 +4510,25 @@
         <v>2047</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>48</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K35" s="20">
         <v>581636686</v>
       </c>
       <c r="Y35" s="13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4519,25 +4536,25 @@
         <v>2048</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>49</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K36" s="20">
         <v>532389478</v>
       </c>
       <c r="Y36" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4545,25 +4562,25 @@
         <v>2049</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K37" s="20">
         <v>501838670</v>
       </c>
       <c r="Y37" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4571,25 +4588,25 @@
         <v>2050</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K38" s="20">
         <v>553324705</v>
       </c>
       <c r="Y38" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4597,28 +4614,28 @@
         <v>2051</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>52</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K39" s="20">
         <v>507665484</v>
       </c>
       <c r="Y39" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4626,28 +4643,28 @@
         <v>2052</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>53</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="K40" s="20">
         <v>536795096</v>
       </c>
       <c r="Y40" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:25" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4655,28 +4672,28 @@
         <v>2053</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="K41" s="6">
         <v>501036561</v>
       </c>
       <c r="Y41" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4684,22 +4701,22 @@
         <v>2054</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>55</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K42" s="20">
         <v>533929525</v>
       </c>
       <c r="Y42" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4707,28 +4724,28 @@
         <v>2055</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>56</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K43" s="20">
         <v>560605311</v>
       </c>
       <c r="Y43" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4736,28 +4753,28 @@
         <v>2056</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>57</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="K44" s="20">
         <v>533151826</v>
       </c>
       <c r="Y44" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4765,25 +4782,25 @@
         <v>2057</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>58</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K45" s="20">
         <v>538205371</v>
       </c>
       <c r="Y45" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4791,28 +4808,28 @@
         <v>2058</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E46" s="13" t="s">
         <v>59</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K46" s="20">
         <v>597658548</v>
       </c>
       <c r="Y46" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:25" s="13" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4820,28 +4837,28 @@
         <v>2059</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>60</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K47" s="20">
         <v>595580288</v>
       </c>
       <c r="Y47" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4849,22 +4866,22 @@
         <v>2060</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>61</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K48" s="20">
         <v>500753444</v>
       </c>
       <c r="Y48" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4872,22 +4889,22 @@
         <v>2061</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>62</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K49" s="20">
         <v>507798916</v>
       </c>
       <c r="Y49" s="13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="50" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4895,28 +4912,28 @@
         <v>2062</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>63</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J50" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="K50" s="20">
         <v>561344457</v>
       </c>
       <c r="Y50" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:25" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4924,25 +4941,25 @@
         <v>2063</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K51" s="6">
         <v>567013115</v>
       </c>
       <c r="Y51" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4950,25 +4967,25 @@
         <v>2064</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E52" s="13" t="s">
         <v>65</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K52" s="20">
         <v>532123164</v>
       </c>
       <c r="Y52" s="13" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="53" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4976,28 +4993,28 @@
         <v>2065</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>66</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="K53" s="20">
         <v>555524996</v>
       </c>
       <c r="Y53" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5005,28 +5022,28 @@
         <v>2066</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E54" s="13" t="s">
         <v>67</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K54" s="20">
         <v>582075735</v>
       </c>
       <c r="Y54" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:25" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5034,25 +5051,25 @@
         <v>2067</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E55" s="13" t="s">
         <v>68</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K55" s="20">
         <v>565424810</v>
       </c>
       <c r="Y55" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5060,28 +5077,28 @@
         <v>2068</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E56" s="13" t="s">
         <v>69</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="K56" s="20">
         <v>503289303</v>
       </c>
       <c r="Y56" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:25" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5089,456 +5106,456 @@
         <v>2069</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K57" s="6"/>
       <c r="Y57" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D58" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E58" s="13" t="s">
         <v>71</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K58" s="20">
         <v>532762609</v>
       </c>
       <c r="Y58" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:25" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D59" s="13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E59" s="13" t="s">
         <v>72</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="K59" s="13">
         <v>547910449</v>
       </c>
       <c r="Y59" s="13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D60" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E60" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K60" s="13">
         <v>595961006</v>
       </c>
       <c r="Y60" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="61" spans="1:25" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D61" s="13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E61" s="13" t="s">
         <v>74</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K61" s="13">
         <v>543847808</v>
       </c>
       <c r="Y61" s="13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D62" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K62" s="2">
         <v>548743509</v>
       </c>
       <c r="Y62" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" spans="1:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D63" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E63" s="11" t="s">
         <v>76</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K63" s="9">
         <v>545393831</v>
       </c>
       <c r="Y63" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D64" s="11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>77</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K64" s="9">
         <v>562140944</v>
       </c>
       <c r="Y64" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D65" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>78</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L65" s="23" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="Y65" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="66" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D66" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>79</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K66" s="9">
         <v>542666542</v>
       </c>
       <c r="Y66" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E67" t="s">
         <v>80</v>
       </c>
       <c r="F67" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G67" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H67" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K67">
         <v>591177100</v>
       </c>
       <c r="Y67" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D68" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>81</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K68" s="9">
         <v>505212231</v>
       </c>
       <c r="Y68" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D69" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>82</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L69" s="10" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="Y69" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D70" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E70" s="9" t="s">
         <v>83</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K70" s="9">
         <v>505506520</v>
       </c>
       <c r="Y70" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D71" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>84</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K71" s="9">
         <v>549146439</v>
       </c>
       <c r="Y71" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D72" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>85</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K72" s="9">
         <v>595020128</v>
       </c>
       <c r="Y72" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="73" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D73" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>86</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H73" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K73" s="9">
         <v>553950176</v>
       </c>
       <c r="Y73" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="74" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D74" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>87</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="K74" s="9">
         <v>501010400</v>
       </c>
       <c r="Y74" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="75" spans="4:25" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D75" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>88</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K75" s="9">
         <v>532732118</v>
       </c>
       <c r="Y75" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="4:25" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D76" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E76" s="9" t="s">
         <v>89</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K76" s="9">
         <v>556369447</v>
       </c>
       <c r="Y76" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="4:25" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D77" s="25" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E77" s="25" t="s">
         <v>90</v>
       </c>
       <c r="F77" s="25" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G77" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H77" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J77" s="25" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="K77" s="25">
         <v>549228994</v>
@@ -5550,19 +5567,19 @@
     </row>
     <row r="78" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D78" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E78" t="s">
         <v>91</v>
       </c>
       <c r="F78" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G78" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H78" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K78">
         <v>500192554</v>
@@ -5574,22 +5591,22 @@
     </row>
     <row r="79" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D79" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E79" t="s">
         <v>92</v>
       </c>
       <c r="F79" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G79" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H79" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J79" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="K79">
         <v>503880000</v>
@@ -5601,22 +5618,22 @@
     </row>
     <row r="80" spans="4:25" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D80" s="13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E80" s="13" t="s">
         <v>93</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G80" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K80" s="13">
         <v>554949955</v>
@@ -5628,22 +5645,22 @@
     </row>
     <row r="81" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E81" t="s">
         <v>94</v>
       </c>
       <c r="F81" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G81" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H81" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J81" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K81">
         <v>506399464</v>
@@ -5655,16 +5672,16 @@
     </row>
     <row r="82" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E82" t="s">
         <v>95</v>
       </c>
       <c r="G82" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H82" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Y82">
         <f t="shared" ca="1" si="0"/>
@@ -5673,22 +5690,22 @@
     </row>
     <row r="83" spans="4:25" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D83" s="25" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E83" s="25" t="s">
         <v>96</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="G83" s="25" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H83" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J83" s="25" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="K83" s="25">
         <v>557652698</v>
@@ -5700,19 +5717,19 @@
     </row>
     <row r="84" spans="4:25" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D84" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E84" s="25" t="s">
         <v>97</v>
       </c>
       <c r="F84" s="25" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H84" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J84" s="25" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K84" s="25">
         <v>581930093</v>
@@ -5724,19 +5741,19 @@
     </row>
     <row r="85" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E85" t="s">
         <v>98</v>
       </c>
       <c r="F85" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H85" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J85" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K85">
         <v>563310927</v>
@@ -5748,13 +5765,13 @@
     </row>
     <row r="86" spans="4:25" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D86" s="25" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E86" s="25" t="s">
         <v>99</v>
       </c>
       <c r="H86" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Y86" s="25">
         <f t="shared" ca="1" si="0"/>
@@ -5763,19 +5780,19 @@
     </row>
     <row r="87" spans="4:25" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D87" s="25" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E87" s="25" t="s">
         <v>100</v>
       </c>
       <c r="F87" s="25" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H87" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J87" s="25" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K87" s="25">
         <v>554000208</v>
@@ -5787,13 +5804,13 @@
     </row>
     <row r="88" spans="4:25" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D88" s="25" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E88" s="25" t="s">
         <v>101</v>
       </c>
       <c r="H88" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Y88" s="25">
         <f t="shared" ca="1" si="0"/>
@@ -5802,13 +5819,13 @@
     </row>
     <row r="89" spans="4:25" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D89" s="25" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E89" s="25" t="s">
         <v>102</v>
       </c>
       <c r="H89" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Y89" s="25">
         <f t="shared" ca="1" si="0"/>
@@ -5817,13 +5834,13 @@
     </row>
     <row r="90" spans="4:25" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D90" s="25" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E90" s="25" t="s">
         <v>103</v>
       </c>
       <c r="H90" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Y90" s="25">
         <f t="shared" ca="1" si="0"/>
@@ -5838,19 +5855,19 @@
     </row>
     <row r="92" spans="4:25" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D92" s="25" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E92" s="25" t="s">
         <v>104</v>
       </c>
       <c r="F92" s="25" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H92" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J92" s="25" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K92" s="25">
         <v>580220982</v>
@@ -5865,16 +5882,16 @@
         <v>105</v>
       </c>
       <c r="F93" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="G93" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H93" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J93" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K93">
         <v>545669065</v>
@@ -5889,16 +5906,16 @@
         <v>85</v>
       </c>
       <c r="F94" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G94" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H94" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J94" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="K94">
         <v>595020128</v>
@@ -5910,25 +5927,25 @@
     </row>
     <row r="95" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D95" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E95" t="s">
         <v>106</v>
       </c>
       <c r="F95" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H95" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J95" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="K95">
         <v>541155533</v>
       </c>
       <c r="L95" s="24" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="Y95">
         <f t="shared" ref="Y95:Y112" ca="1" si="1">A94:Y115</f>
@@ -5937,19 +5954,19 @@
     </row>
     <row r="96" spans="4:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D96" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E96" t="s">
         <v>107</v>
       </c>
       <c r="F96" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H96" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J96" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K96">
         <v>506503636</v>
@@ -5961,16 +5978,16 @@
     </row>
     <row r="97" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D97" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E97" t="s">
         <v>108</v>
       </c>
       <c r="F97" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="J97" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="K97">
         <v>593777790</v>
@@ -5982,16 +5999,16 @@
     </row>
     <row r="98" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D98" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E98" t="s">
         <v>109</v>
       </c>
       <c r="F98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J98" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K98">
         <v>556622716</v>
@@ -6003,7 +6020,7 @@
     </row>
     <row r="99" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D99" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E99" t="s">
         <v>110</v>
@@ -6015,19 +6032,19 @@
     </row>
     <row r="100" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D100" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E100" t="s">
         <v>111</v>
       </c>
       <c r="F100" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="H100" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J100" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="K100">
         <v>534859217</v>
@@ -6039,25 +6056,25 @@
     </row>
     <row r="101" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D101" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E101" t="s">
         <v>112</v>
       </c>
       <c r="F101" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H101" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J101" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="K101">
         <v>592482486</v>
       </c>
       <c r="L101" s="24" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="Y101">
         <f t="shared" ca="1" si="1"/>
@@ -6066,16 +6083,16 @@
     </row>
     <row r="102" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D102" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E102" t="s">
         <v>113</v>
       </c>
       <c r="F102" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="J102" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K102">
         <v>506486949</v>
@@ -6087,19 +6104,19 @@
     </row>
     <row r="103" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D103" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E103" t="s">
         <v>114</v>
       </c>
       <c r="F103" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H103" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J103" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="K103">
         <v>500800864</v>
@@ -6114,16 +6131,16 @@
         <v>0</v>
       </c>
       <c r="D104" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E104" t="s">
         <v>115</v>
       </c>
       <c r="F104" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="J104" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K104">
         <v>508887437</v>
@@ -6135,25 +6152,25 @@
     </row>
     <row r="105" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D105" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E105" t="s">
         <v>116</v>
       </c>
       <c r="F105" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="H105" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J105" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="K105">
         <v>560071794</v>
       </c>
       <c r="L105" s="24" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="Y105">
         <f t="shared" ca="1" si="1"/>
@@ -6162,16 +6179,16 @@
     </row>
     <row r="106" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D106" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E106" t="s">
         <v>117</v>
       </c>
       <c r="F106" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="J106" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="K106">
         <v>504544073</v>
@@ -6183,19 +6200,19 @@
     </row>
     <row r="107" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D107" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E107" t="s">
         <v>118</v>
       </c>
       <c r="F107" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H107" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J107" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K107">
         <v>503674125</v>
@@ -6207,25 +6224,25 @@
     </row>
     <row r="108" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D108" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E108" t="s">
         <v>119</v>
       </c>
       <c r="F108" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="H108" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J108" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K108">
         <v>561161461</v>
       </c>
       <c r="L108" s="24" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="Y108">
         <f t="shared" ca="1" si="1"/>
@@ -6234,25 +6251,25 @@
     </row>
     <row r="109" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D109" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E109" t="s">
         <v>120</v>
       </c>
       <c r="F109" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H109" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J109" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K109">
         <v>500188766</v>
       </c>
       <c r="L109" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="Y109">
         <f t="shared" ca="1" si="1"/>
@@ -6261,16 +6278,16 @@
     </row>
     <row r="110" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D110" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="E110" t="s">
-        <v>348</v>
+        <v>121</v>
       </c>
       <c r="F110" t="s">
         <v>349</v>
       </c>
       <c r="J110" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K110">
         <v>560957508</v>
@@ -6494,10 +6511,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A4C288-A87C-49B3-B1E5-1AA21A4B10B3}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6551,6 +6568,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B4" s="8">
+        <v>45960</v>
+      </c>
       <c r="G4">
         <v>62</v>
       </c>
@@ -6580,6 +6603,86 @@
       </c>
       <c r="H7" s="8">
         <v>45946</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>70</v>
+      </c>
+      <c r="H8" s="8">
+        <v>45949</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>56</v>
+      </c>
+      <c r="H9" s="8">
+        <v>45950</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>58</v>
+      </c>
+      <c r="H10" s="8">
+        <v>45951</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>61</v>
+      </c>
+      <c r="H11" s="8">
+        <v>45952</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>64</v>
+      </c>
+      <c r="H12" s="8">
+        <v>45953</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>52</v>
+      </c>
+      <c r="H13" s="8">
+        <v>45956</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>59</v>
+      </c>
+      <c r="H14" s="8">
+        <v>45957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>63</v>
+      </c>
+      <c r="H15" s="8">
+        <v>45958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>52</v>
+      </c>
+      <c r="H16" s="8">
+        <v>45959</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>58</v>
+      </c>
+      <c r="H17" s="8">
+        <v>45960</v>
       </c>
     </row>
   </sheetData>

</xml_diff>